<commit_message>
web 122 / quiz 02
</commit_message>
<xml_diff>
--- a/122/122.xlsx
+++ b/122/122.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\MFT\004-scores\122\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F58D45C9-DE9E-445C-8736-842C7E6E6B6C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BAA6C8A-7044-4E8C-8B37-4685A98CBD89}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3135" yWindow="2640" windowWidth="21600" windowHeight="11385" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="web 120" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="9">
   <si>
     <t>No.</t>
   </si>
@@ -56,6 +56,9 @@
   </si>
   <si>
     <t>MFT</t>
+  </si>
+  <si>
+    <t>Q02</t>
   </si>
 </sst>
 </file>
@@ -566,7 +569,7 @@
   <dimension ref="A1:Z37"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -592,7 +595,9 @@
       <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2"/>
+      <c r="C1" s="2" t="s">
+        <v>8</v>
+      </c>
       <c r="D1" s="2"/>
       <c r="E1" s="2"/>
       <c r="F1" s="2"/>
@@ -616,7 +621,10 @@
         <f>(7/10)*10</f>
         <v>7</v>
       </c>
-      <c r="C2" s="4"/>
+      <c r="C2" s="4">
+        <f>(21/25)*10</f>
+        <v>8.4</v>
+      </c>
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
       <c r="F2" s="4"/>
@@ -649,7 +657,10 @@
         <f>(9/10)*10</f>
         <v>9</v>
       </c>
-      <c r="C3" s="4"/>
+      <c r="C3" s="4">
+        <f>(18/25)*10</f>
+        <v>7.1999999999999993</v>
+      </c>
       <c r="D3" s="4"/>
       <c r="E3" s="4"/>
       <c r="F3" s="4"/>
@@ -682,7 +693,10 @@
         <f>(9/10)*10</f>
         <v>9</v>
       </c>
-      <c r="C4" s="4"/>
+      <c r="C4" s="4">
+        <f>(21/25)*10</f>
+        <v>8.4</v>
+      </c>
       <c r="D4" s="4"/>
       <c r="E4" s="4"/>
       <c r="F4" s="4"/>
@@ -715,7 +729,10 @@
         <f>(7/10)*10</f>
         <v>7</v>
       </c>
-      <c r="C5" s="4"/>
+      <c r="C5" s="4">
+        <f>(22/25)*10</f>
+        <v>8.8000000000000007</v>
+      </c>
       <c r="D5" s="4"/>
       <c r="E5" s="4"/>
       <c r="F5" s="4"/>
@@ -747,7 +764,10 @@
       <c r="B6" s="6">
         <v>10</v>
       </c>
-      <c r="C6" s="4"/>
+      <c r="C6" s="4">
+        <f>(23/25)*10</f>
+        <v>9.2000000000000011</v>
+      </c>
       <c r="D6" s="4"/>
       <c r="E6" s="4"/>
       <c r="F6" s="4"/>
@@ -779,7 +799,10 @@
       <c r="B7" s="6">
         <v>9</v>
       </c>
-      <c r="C7" s="6"/>
+      <c r="C7" s="6">
+        <f>(24/25)*10</f>
+        <v>9.6</v>
+      </c>
       <c r="D7" s="6"/>
       <c r="E7" s="6"/>
       <c r="F7" s="6"/>
@@ -811,7 +834,10 @@
       <c r="B8" s="6">
         <v>10</v>
       </c>
-      <c r="C8" s="6"/>
+      <c r="C8" s="6">
+        <f>(22/25)*10</f>
+        <v>8.8000000000000007</v>
+      </c>
       <c r="D8" s="6"/>
       <c r="E8" s="6"/>
       <c r="F8" s="6"/>
@@ -843,7 +869,10 @@
       <c r="B9" s="6">
         <v>4</v>
       </c>
-      <c r="C9" s="6"/>
+      <c r="C9" s="6">
+        <f>(15/25)*10</f>
+        <v>6</v>
+      </c>
       <c r="D9" s="6"/>
       <c r="E9" s="6"/>
       <c r="F9" s="6"/>
@@ -875,7 +904,10 @@
       <c r="B10" s="6">
         <v>7</v>
       </c>
-      <c r="C10" s="6"/>
+      <c r="C10" s="6">
+        <f>(21/25)*10</f>
+        <v>8.4</v>
+      </c>
       <c r="D10" s="6"/>
       <c r="E10" s="6"/>
       <c r="F10" s="6"/>
@@ -907,7 +939,10 @@
       <c r="B11" s="6">
         <v>6</v>
       </c>
-      <c r="C11" s="6"/>
+      <c r="C11" s="6">
+        <f>(15/25)*10</f>
+        <v>6</v>
+      </c>
       <c r="D11" s="6"/>
       <c r="E11" s="6"/>
       <c r="F11" s="6"/>
@@ -939,7 +974,10 @@
       <c r="B12" s="6">
         <v>5</v>
       </c>
-      <c r="C12" s="6"/>
+      <c r="C12" s="6">
+        <f>(21/25)*10</f>
+        <v>8.4</v>
+      </c>
       <c r="D12" s="6"/>
       <c r="E12" s="6"/>
       <c r="F12" s="6"/>
@@ -1086,7 +1124,7 @@
       </c>
       <c r="B17" s="8">
         <f>COUNTA(B1:Q1) * 10</f>
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="C17" s="5"/>
       <c r="D17" s="5"/>
@@ -1144,7 +1182,7 @@
       </c>
       <c r="B22" s="13">
         <f>(SUM(B2:R2)/B17) * 40</f>
-        <v>28</v>
+        <v>30.8</v>
       </c>
       <c r="C22" s="14">
         <v>0</v>
@@ -1154,11 +1192,11 @@
       </c>
       <c r="E22" s="15">
         <f>B22+C22+D22</f>
-        <v>28</v>
+        <v>30.8</v>
       </c>
       <c r="F22" s="16">
-        <f t="shared" ref="F22:F36" si="0">E22</f>
-        <v>28</v>
+        <f t="shared" ref="F22:F33" si="0">E22</f>
+        <v>30.8</v>
       </c>
     </row>
     <row r="23" spans="1:26" x14ac:dyDescent="0.25">
@@ -1167,7 +1205,7 @@
       </c>
       <c r="B23" s="13">
         <f>(SUM(B3:R3)/B17) * 40</f>
-        <v>36</v>
+        <v>32.4</v>
       </c>
       <c r="C23" s="14">
         <v>0</v>
@@ -1176,12 +1214,12 @@
         <v>0</v>
       </c>
       <c r="E23" s="15">
-        <f t="shared" ref="E23:E36" si="1">B23+C23+D23</f>
-        <v>36</v>
+        <f t="shared" ref="E23:E33" si="1">B23+C23+D23</f>
+        <v>32.4</v>
       </c>
       <c r="F23" s="16">
         <f t="shared" si="0"/>
-        <v>36</v>
+        <v>32.4</v>
       </c>
     </row>
     <row r="24" spans="1:26" x14ac:dyDescent="0.25">
@@ -1190,7 +1228,7 @@
       </c>
       <c r="B24" s="13">
         <f>(SUM(B4:R4)/B17) * 40</f>
-        <v>36</v>
+        <v>34.799999999999997</v>
       </c>
       <c r="C24" s="14">
         <v>0</v>
@@ -1200,11 +1238,11 @@
       </c>
       <c r="E24" s="15">
         <f t="shared" si="1"/>
-        <v>36</v>
+        <v>34.799999999999997</v>
       </c>
       <c r="F24" s="16">
         <f t="shared" si="0"/>
-        <v>36</v>
+        <v>34.799999999999997</v>
       </c>
     </row>
     <row r="25" spans="1:26" x14ac:dyDescent="0.25">
@@ -1213,7 +1251,7 @@
       </c>
       <c r="B25" s="13">
         <f>(SUM(B5:R5)/B17) * 40</f>
-        <v>28</v>
+        <v>31.6</v>
       </c>
       <c r="C25" s="14">
         <v>0</v>
@@ -1223,11 +1261,11 @@
       </c>
       <c r="E25" s="15">
         <f t="shared" si="1"/>
-        <v>28</v>
+        <v>31.6</v>
       </c>
       <c r="F25" s="16">
         <f t="shared" si="0"/>
-        <v>28</v>
+        <v>31.6</v>
       </c>
     </row>
     <row r="26" spans="1:26" x14ac:dyDescent="0.25">
@@ -1236,7 +1274,7 @@
       </c>
       <c r="B26" s="13">
         <f>(SUM(B6:R6)/B17) * 40</f>
-        <v>40</v>
+        <v>38.400000000000006</v>
       </c>
       <c r="C26" s="14">
         <v>0</v>
@@ -1246,11 +1284,11 @@
       </c>
       <c r="E26" s="15">
         <f t="shared" si="1"/>
-        <v>40</v>
+        <v>38.400000000000006</v>
       </c>
       <c r="F26" s="16">
         <f t="shared" si="0"/>
-        <v>40</v>
+        <v>38.400000000000006</v>
       </c>
     </row>
     <row r="27" spans="1:26" x14ac:dyDescent="0.25">
@@ -1259,7 +1297,7 @@
       </c>
       <c r="B27" s="13">
         <f>(SUM(B7:R7)/B17) * 40</f>
-        <v>36</v>
+        <v>37.200000000000003</v>
       </c>
       <c r="C27" s="14">
         <v>0</v>
@@ -1269,11 +1307,11 @@
       </c>
       <c r="E27" s="15">
         <f t="shared" si="1"/>
-        <v>36</v>
+        <v>37.200000000000003</v>
       </c>
       <c r="F27" s="16">
         <f t="shared" si="0"/>
-        <v>36</v>
+        <v>37.200000000000003</v>
       </c>
     </row>
     <row r="28" spans="1:26" x14ac:dyDescent="0.25">
@@ -1282,7 +1320,7 @@
       </c>
       <c r="B28" s="13">
         <f>(SUM(B8:R8)/B17) * 40</f>
-        <v>40</v>
+        <v>37.6</v>
       </c>
       <c r="C28" s="14">
         <v>0</v>
@@ -1292,11 +1330,11 @@
       </c>
       <c r="E28" s="15">
         <f t="shared" si="1"/>
-        <v>40</v>
+        <v>37.6</v>
       </c>
       <c r="F28" s="16">
         <f t="shared" si="0"/>
-        <v>40</v>
+        <v>37.6</v>
       </c>
     </row>
     <row r="29" spans="1:26" x14ac:dyDescent="0.25">
@@ -1305,7 +1343,7 @@
       </c>
       <c r="B29" s="13">
         <f>(SUM(B9:R9)/B17) * 40</f>
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="C29" s="14">
         <v>0</v>
@@ -1315,11 +1353,11 @@
       </c>
       <c r="E29" s="15">
         <f t="shared" si="1"/>
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="F29" s="16">
         <f t="shared" si="0"/>
-        <v>16</v>
+        <v>20</v>
       </c>
     </row>
     <row r="30" spans="1:26" x14ac:dyDescent="0.25">
@@ -1328,7 +1366,7 @@
       </c>
       <c r="B30" s="13">
         <f>(SUM(B10:R10)/B17) * 40</f>
-        <v>28</v>
+        <v>30.8</v>
       </c>
       <c r="C30" s="14">
         <v>0</v>
@@ -1338,11 +1376,11 @@
       </c>
       <c r="E30" s="15">
         <f t="shared" si="1"/>
-        <v>28</v>
+        <v>30.8</v>
       </c>
       <c r="F30" s="16">
         <f t="shared" si="0"/>
-        <v>28</v>
+        <v>30.8</v>
       </c>
     </row>
     <row r="31" spans="1:26" x14ac:dyDescent="0.25">
@@ -1374,7 +1412,7 @@
       </c>
       <c r="B32" s="13">
         <f>(SUM(B12:R12)/B17) * 40</f>
-        <v>20</v>
+        <v>26.8</v>
       </c>
       <c r="C32" s="14">
         <v>0</v>
@@ -1384,11 +1422,11 @@
       </c>
       <c r="E32" s="15">
         <f t="shared" si="1"/>
-        <v>20</v>
+        <v>26.8</v>
       </c>
       <c r="F32" s="16">
         <f t="shared" si="0"/>
-        <v>20</v>
+        <v>26.8</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
web 122 / updated
</commit_message>
<xml_diff>
--- a/122/122.xlsx
+++ b/122/122.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\MFT\004-scores\122\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BAA6C8A-7044-4E8C-8B37-4685A98CBD89}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F6F701D-9D31-4EEB-8558-06B534DA88EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="13">
   <si>
     <t>No.</t>
   </si>
@@ -60,12 +60,24 @@
   <si>
     <t>Q02</t>
   </si>
+  <si>
+    <t>H01</t>
+  </si>
+  <si>
+    <t>H02</t>
+  </si>
+  <si>
+    <t>H05</t>
+  </si>
+  <si>
+    <t>H06</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -76,6 +88,12 @@
     <font>
       <sz val="11"/>
       <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
@@ -569,7 +587,7 @@
   <dimension ref="A1:Z37"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="D32" sqref="D32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -598,10 +616,18 @@
       <c r="C1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2"/>
+      <c r="D1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>12</v>
+      </c>
       <c r="H1" s="2"/>
       <c r="I1" s="2"/>
       <c r="J1" s="2"/>
@@ -625,10 +651,18 @@
         <f>(21/25)*10</f>
         <v>8.4</v>
       </c>
-      <c r="D2" s="4"/>
-      <c r="E2" s="4"/>
-      <c r="F2" s="4"/>
-      <c r="G2" s="4"/>
+      <c r="D2" s="4">
+        <v>10</v>
+      </c>
+      <c r="E2" s="4">
+        <v>9.5</v>
+      </c>
+      <c r="F2" s="4">
+        <v>10</v>
+      </c>
+      <c r="G2" s="4">
+        <v>9.5</v>
+      </c>
       <c r="H2" s="4"/>
       <c r="I2" s="4"/>
       <c r="J2" s="4"/>
@@ -661,10 +695,18 @@
         <f>(18/25)*10</f>
         <v>7.1999999999999993</v>
       </c>
-      <c r="D3" s="4"/>
-      <c r="E3" s="4"/>
-      <c r="F3" s="4"/>
-      <c r="G3" s="4"/>
+      <c r="D3" s="4">
+        <v>10</v>
+      </c>
+      <c r="E3" s="4">
+        <v>9.75</v>
+      </c>
+      <c r="F3" s="4">
+        <v>10</v>
+      </c>
+      <c r="G3" s="4">
+        <v>10</v>
+      </c>
       <c r="H3" s="4"/>
       <c r="I3" s="4"/>
       <c r="J3" s="4"/>
@@ -697,10 +739,18 @@
         <f>(21/25)*10</f>
         <v>8.4</v>
       </c>
-      <c r="D4" s="4"/>
-      <c r="E4" s="4"/>
-      <c r="F4" s="4"/>
-      <c r="G4" s="4"/>
+      <c r="D4" s="4">
+        <v>10</v>
+      </c>
+      <c r="E4" s="4">
+        <v>9.75</v>
+      </c>
+      <c r="F4" s="4">
+        <v>10</v>
+      </c>
+      <c r="G4" s="4">
+        <v>9.5</v>
+      </c>
       <c r="H4" s="4"/>
       <c r="I4" s="4"/>
       <c r="J4" s="4"/>
@@ -733,10 +783,18 @@
         <f>(22/25)*10</f>
         <v>8.8000000000000007</v>
       </c>
-      <c r="D5" s="4"/>
-      <c r="E5" s="4"/>
-      <c r="F5" s="4"/>
-      <c r="G5" s="4"/>
+      <c r="D5" s="4">
+        <v>10</v>
+      </c>
+      <c r="E5" s="4">
+        <v>9.5</v>
+      </c>
+      <c r="F5" s="4">
+        <v>10</v>
+      </c>
+      <c r="G5" s="4">
+        <v>9</v>
+      </c>
       <c r="H5" s="4"/>
       <c r="I5" s="4"/>
       <c r="J5" s="4"/>
@@ -768,10 +826,18 @@
         <f>(23/25)*10</f>
         <v>9.2000000000000011</v>
       </c>
-      <c r="D6" s="4"/>
-      <c r="E6" s="4"/>
-      <c r="F6" s="4"/>
-      <c r="G6" s="4"/>
+      <c r="D6" s="4">
+        <v>10</v>
+      </c>
+      <c r="E6" s="4">
+        <v>9.75</v>
+      </c>
+      <c r="F6" s="4">
+        <v>10</v>
+      </c>
+      <c r="G6" s="4">
+        <v>9.5</v>
+      </c>
       <c r="H6" s="4"/>
       <c r="I6" s="4"/>
       <c r="J6" s="4"/>
@@ -803,10 +869,18 @@
         <f>(24/25)*10</f>
         <v>9.6</v>
       </c>
-      <c r="D7" s="6"/>
-      <c r="E7" s="6"/>
-      <c r="F7" s="6"/>
-      <c r="G7" s="6"/>
+      <c r="D7" s="6">
+        <v>10</v>
+      </c>
+      <c r="E7" s="6">
+        <v>10</v>
+      </c>
+      <c r="F7" s="6">
+        <v>10</v>
+      </c>
+      <c r="G7" s="6">
+        <v>9</v>
+      </c>
       <c r="H7" s="6"/>
       <c r="I7" s="6"/>
       <c r="J7" s="6"/>
@@ -838,10 +912,18 @@
         <f>(22/25)*10</f>
         <v>8.8000000000000007</v>
       </c>
-      <c r="D8" s="6"/>
-      <c r="E8" s="6"/>
-      <c r="F8" s="6"/>
-      <c r="G8" s="6"/>
+      <c r="D8" s="6">
+        <v>10.5</v>
+      </c>
+      <c r="E8" s="6">
+        <v>10</v>
+      </c>
+      <c r="F8" s="6">
+        <v>10</v>
+      </c>
+      <c r="G8" s="6">
+        <v>10</v>
+      </c>
       <c r="H8" s="6"/>
       <c r="I8" s="6"/>
       <c r="J8" s="6"/>
@@ -873,10 +955,18 @@
         <f>(15/25)*10</f>
         <v>6</v>
       </c>
-      <c r="D9" s="6"/>
-      <c r="E9" s="6"/>
-      <c r="F9" s="6"/>
-      <c r="G9" s="6"/>
+      <c r="D9" s="6">
+        <v>9</v>
+      </c>
+      <c r="E9" s="6">
+        <v>9.5</v>
+      </c>
+      <c r="F9" s="6">
+        <v>9</v>
+      </c>
+      <c r="G9" s="6">
+        <v>10</v>
+      </c>
       <c r="H9" s="6"/>
       <c r="I9" s="6"/>
       <c r="J9" s="6"/>
@@ -908,10 +998,18 @@
         <f>(21/25)*10</f>
         <v>8.4</v>
       </c>
-      <c r="D10" s="6"/>
-      <c r="E10" s="6"/>
-      <c r="F10" s="6"/>
-      <c r="G10" s="6"/>
+      <c r="D10" s="6">
+        <v>9</v>
+      </c>
+      <c r="E10" s="6">
+        <v>10.5</v>
+      </c>
+      <c r="F10" s="6">
+        <v>10</v>
+      </c>
+      <c r="G10" s="6">
+        <v>9</v>
+      </c>
       <c r="H10" s="6"/>
       <c r="I10" s="6"/>
       <c r="J10" s="6"/>
@@ -943,10 +1041,18 @@
         <f>(15/25)*10</f>
         <v>6</v>
       </c>
-      <c r="D11" s="6"/>
-      <c r="E11" s="6"/>
-      <c r="F11" s="6"/>
-      <c r="G11" s="6"/>
+      <c r="D11" s="6">
+        <v>10</v>
+      </c>
+      <c r="E11" s="6">
+        <v>9</v>
+      </c>
+      <c r="F11" s="6">
+        <v>10</v>
+      </c>
+      <c r="G11" s="6">
+        <v>10</v>
+      </c>
       <c r="H11" s="6"/>
       <c r="I11" s="6"/>
       <c r="J11" s="6"/>
@@ -978,10 +1084,18 @@
         <f>(21/25)*10</f>
         <v>8.4</v>
       </c>
-      <c r="D12" s="6"/>
-      <c r="E12" s="6"/>
-      <c r="F12" s="6"/>
-      <c r="G12" s="6"/>
+      <c r="D12" s="6">
+        <v>9.75</v>
+      </c>
+      <c r="E12" s="6">
+        <v>9.5</v>
+      </c>
+      <c r="F12" s="6">
+        <v>9</v>
+      </c>
+      <c r="G12" s="6">
+        <v>9.5</v>
+      </c>
       <c r="H12" s="6"/>
       <c r="I12" s="6"/>
       <c r="J12" s="6"/>
@@ -1003,12 +1117,8 @@
       <c r="Z12" s="5"/>
     </row>
     <row r="13" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A13" s="3">
-        <v>16</v>
-      </c>
-      <c r="B13" s="6">
-        <v>0</v>
-      </c>
+      <c r="A13" s="3"/>
+      <c r="B13" s="6"/>
       <c r="C13" s="6"/>
       <c r="D13" s="4"/>
       <c r="E13" s="6"/>
@@ -1124,7 +1234,7 @@
       </c>
       <c r="B17" s="8">
         <f>COUNTA(B1:Q1) * 10</f>
-        <v>20</v>
+        <v>60</v>
       </c>
       <c r="C17" s="5"/>
       <c r="D17" s="5"/>
@@ -1182,21 +1292,21 @@
       </c>
       <c r="B22" s="13">
         <f>(SUM(B2:R2)/B17) * 40</f>
-        <v>30.8</v>
+        <v>36.266666666666666</v>
       </c>
       <c r="C22" s="14">
-        <v>0</v>
+        <v>9.5</v>
       </c>
       <c r="D22" s="14">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="E22" s="15">
         <f>B22+C22+D22</f>
-        <v>30.8</v>
+        <v>95.766666666666666</v>
       </c>
       <c r="F22" s="16">
         <f t="shared" ref="F22:F33" si="0">E22</f>
-        <v>30.8</v>
+        <v>95.766666666666666</v>
       </c>
     </row>
     <row r="23" spans="1:26" x14ac:dyDescent="0.25">
@@ -1205,21 +1315,21 @@
       </c>
       <c r="B23" s="13">
         <f>(SUM(B3:R3)/B17) * 40</f>
-        <v>32.4</v>
+        <v>37.299999999999997</v>
       </c>
       <c r="C23" s="14">
-        <v>0</v>
+        <v>9.5</v>
       </c>
       <c r="D23" s="14">
-        <v>0</v>
+        <v>55</v>
       </c>
       <c r="E23" s="15">
         <f t="shared" ref="E23:E33" si="1">B23+C23+D23</f>
-        <v>32.4</v>
+        <v>101.8</v>
       </c>
       <c r="F23" s="16">
         <f t="shared" si="0"/>
-        <v>32.4</v>
+        <v>101.8</v>
       </c>
     </row>
     <row r="24" spans="1:26" x14ac:dyDescent="0.25">
@@ -1228,21 +1338,21 @@
       </c>
       <c r="B24" s="13">
         <f>(SUM(B4:R4)/B17) * 40</f>
-        <v>34.799999999999997</v>
+        <v>37.766666666666666</v>
       </c>
       <c r="C24" s="14">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="D24" s="14">
-        <v>0</v>
+        <v>55</v>
       </c>
       <c r="E24" s="15">
         <f t="shared" si="1"/>
-        <v>34.799999999999997</v>
+        <v>102.76666666666667</v>
       </c>
       <c r="F24" s="16">
         <f t="shared" si="0"/>
-        <v>34.799999999999997</v>
+        <v>102.76666666666667</v>
       </c>
     </row>
     <row r="25" spans="1:26" x14ac:dyDescent="0.25">
@@ -1251,21 +1361,21 @@
       </c>
       <c r="B25" s="13">
         <f>(SUM(B5:R5)/B17) * 40</f>
-        <v>31.6</v>
+        <v>36.199999999999996</v>
       </c>
       <c r="C25" s="14">
-        <v>0</v>
+        <v>9.5</v>
       </c>
       <c r="D25" s="14">
-        <v>0</v>
+        <v>45</v>
       </c>
       <c r="E25" s="15">
         <f t="shared" si="1"/>
-        <v>31.6</v>
+        <v>90.699999999999989</v>
       </c>
       <c r="F25" s="16">
         <f t="shared" si="0"/>
-        <v>31.6</v>
+        <v>90.699999999999989</v>
       </c>
     </row>
     <row r="26" spans="1:26" x14ac:dyDescent="0.25">
@@ -1274,21 +1384,21 @@
       </c>
       <c r="B26" s="13">
         <f>(SUM(B6:R6)/B17) * 40</f>
-        <v>38.400000000000006</v>
+        <v>38.966666666666669</v>
       </c>
       <c r="C26" s="14">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="D26" s="14">
-        <v>0</v>
+        <v>59</v>
       </c>
       <c r="E26" s="15">
         <f t="shared" si="1"/>
-        <v>38.400000000000006</v>
+        <v>107.96666666666667</v>
       </c>
       <c r="F26" s="16">
         <f t="shared" si="0"/>
-        <v>38.400000000000006</v>
+        <v>107.96666666666667</v>
       </c>
     </row>
     <row r="27" spans="1:26" x14ac:dyDescent="0.25">
@@ -1297,21 +1407,21 @@
       </c>
       <c r="B27" s="13">
         <f>(SUM(B7:R7)/B17) * 40</f>
-        <v>37.200000000000003</v>
+        <v>38.400000000000006</v>
       </c>
       <c r="C27" s="14">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="D27" s="14">
-        <v>0</v>
+        <v>60</v>
       </c>
       <c r="E27" s="15">
         <f t="shared" si="1"/>
-        <v>37.200000000000003</v>
+        <v>108.4</v>
       </c>
       <c r="F27" s="16">
         <f t="shared" si="0"/>
-        <v>37.200000000000003</v>
+        <v>108.4</v>
       </c>
     </row>
     <row r="28" spans="1:26" x14ac:dyDescent="0.25">
@@ -1320,21 +1430,21 @@
       </c>
       <c r="B28" s="13">
         <f>(SUM(B8:R8)/B17) * 40</f>
-        <v>37.6</v>
+        <v>39.533333333333331</v>
       </c>
       <c r="C28" s="14">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="D28" s="14">
-        <v>0</v>
+        <v>60</v>
       </c>
       <c r="E28" s="15">
         <f t="shared" si="1"/>
-        <v>37.6</v>
+        <v>109.53333333333333</v>
       </c>
       <c r="F28" s="16">
         <f t="shared" si="0"/>
-        <v>37.6</v>
+        <v>109.53333333333333</v>
       </c>
     </row>
     <row r="29" spans="1:26" x14ac:dyDescent="0.25">
@@ -1343,21 +1453,21 @@
       </c>
       <c r="B29" s="13">
         <f>(SUM(B9:R9)/B17) * 40</f>
-        <v>20</v>
+        <v>31.666666666666664</v>
       </c>
       <c r="C29" s="14">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="D29" s="14">
         <v>0</v>
       </c>
       <c r="E29" s="15">
         <f t="shared" si="1"/>
-        <v>20</v>
+        <v>40.666666666666664</v>
       </c>
       <c r="F29" s="16">
         <f t="shared" si="0"/>
-        <v>20</v>
+        <v>40.666666666666664</v>
       </c>
     </row>
     <row r="30" spans="1:26" x14ac:dyDescent="0.25">
@@ -1366,21 +1476,21 @@
       </c>
       <c r="B30" s="13">
         <f>(SUM(B10:R10)/B17) * 40</f>
-        <v>30.8</v>
+        <v>35.93333333333333</v>
       </c>
       <c r="C30" s="14">
-        <v>0</v>
+        <v>9.5</v>
       </c>
       <c r="D30" s="14">
         <v>0</v>
       </c>
       <c r="E30" s="15">
         <f t="shared" si="1"/>
-        <v>30.8</v>
+        <v>45.43333333333333</v>
       </c>
       <c r="F30" s="16">
         <f t="shared" si="0"/>
-        <v>30.8</v>
+        <v>45.43333333333333</v>
       </c>
     </row>
     <row r="31" spans="1:26" x14ac:dyDescent="0.25">
@@ -1389,21 +1499,21 @@
       </c>
       <c r="B31" s="13">
         <f>(SUM(B11:R11)/B17) * 40</f>
-        <v>24</v>
+        <v>34</v>
       </c>
       <c r="C31" s="14">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="D31" s="14">
         <v>0</v>
       </c>
       <c r="E31" s="15">
         <f t="shared" si="1"/>
-        <v>24</v>
+        <v>44</v>
       </c>
       <c r="F31" s="16">
         <f t="shared" si="0"/>
-        <v>24</v>
+        <v>44</v>
       </c>
     </row>
     <row r="32" spans="1:26" x14ac:dyDescent="0.25">
@@ -1412,45 +1522,30 @@
       </c>
       <c r="B32" s="13">
         <f>(SUM(B12:R12)/B17) * 40</f>
-        <v>26.8</v>
+        <v>34.099999999999994</v>
       </c>
       <c r="C32" s="14">
-        <v>0</v>
+        <v>9.5</v>
       </c>
       <c r="D32" s="14">
         <v>0</v>
       </c>
       <c r="E32" s="15">
         <f t="shared" si="1"/>
-        <v>26.8</v>
+        <v>43.599999999999994</v>
       </c>
       <c r="F32" s="16">
         <f t="shared" si="0"/>
-        <v>26.8</v>
+        <v>43.599999999999994</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A33" s="10">
-        <v>16</v>
-      </c>
-      <c r="B33" s="13">
-        <f>(SUM(B13:R13)/B17) * 40</f>
-        <v>0</v>
-      </c>
-      <c r="C33" s="14">
-        <v>0</v>
-      </c>
-      <c r="D33" s="14">
-        <v>0</v>
-      </c>
-      <c r="E33" s="15">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="F33" s="16">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
+      <c r="A33" s="10"/>
+      <c r="B33" s="13"/>
+      <c r="C33" s="14"/>
+      <c r="D33" s="14"/>
+      <c r="E33" s="15"/>
+      <c r="F33" s="16"/>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" s="19"/>
@@ -1480,6 +1575,7 @@
       <c r="A37" s="17"/>
     </row>
   </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>

</xml_diff>